<commit_message>
Extend readme, add hardware & firmware instructions
</commit_message>
<xml_diff>
--- a/firmware/configs/llnl001.xlsx
+++ b/firmware/configs/llnl001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="pinouts" sheetId="1" state="visible" r:id="rId2"/>
@@ -331,11 +331,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="16.3"/>
@@ -891,7 +891,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -906,11 +906,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.3"/>
@@ -1198,7 +1198,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>